<commit_message>
Updated Eagle files + BOMs
</commit_message>
<xml_diff>
--- a/BOMs/Glint module BOM.xlsx
+++ b/BOMs/Glint module BOM.xlsx
@@ -472,7 +472,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,14 +577,14 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>0.56000000000000005</v>
       </c>
       <c r="F4" s="3">
         <f>D4*E4</f>
-        <v>1.1200000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -599,7 +599,7 @@
       </c>
       <c r="F6" s="3">
         <f>SUM(F2:F4)</f>
-        <v>4.6896000000000004</v>
+        <v>4.1295999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>